<commit_message>
Fix legend misalignment in thumbnail images
Legend colors were out of sync with bar colors in thumbnail images due to error in legend label manipulation.  Fixed that problem and regenerated charts.  Also changed MoreInformationURL to point to the correct asset on SharePoint.  Apparent changes to output data are only due to changed order of records.  No meaningful changes.
</commit_message>
<xml_diff>
--- a/output_data/charts/0500000US39041.xlsx
+++ b/output_data/charts/0500000US39041.xlsx
@@ -162,7 +162,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="BCBD22"/>
+              <a:srgbClr val="FF7F0E"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -353,7 +353,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="7F7F7F"/>
+              <a:srgbClr val="2CA02C"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -538,6 +538,579 @@
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>Electric</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="D62728"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ethanol (E85)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="9467BD"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hydrogen</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="8C564B"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Liquefied Natural Gas (LNG)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -636,579 +1209,6 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ethanol (E85)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="8C564B"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
-                <c:pt idx="0">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2018</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2019</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2020</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2021</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2022</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2023</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2024</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$E$2:$E$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Hydrogen</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="9467BD"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
-                <c:pt idx="0">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2018</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2019</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2020</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2021</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2022</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2023</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2024</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$F$2:$F$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Liquefied Natural Gas (LNG)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="D62728"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
-                <c:pt idx="0">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2018</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2019</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2020</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2021</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2022</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2023</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2024</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
               <c:f>Sheet1!$G$2:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1308,7 +1308,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="2CA02C"/>
+              <a:srgbClr val="7F7F7F"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>

</xml_diff>